<commit_message>
App and Link objects
</commit_message>
<xml_diff>
--- a/Content/SailPoint_IIQ_Object_API.xlsx
+++ b/Content/SailPoint_IIQ_Object_API.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SailPoint\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SailPoint\Content\SailPoint-IIQ\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A062F521-452E-48F5-BC2E-0DD8FB268AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED34EC8-B9B2-45CE-9284-DEEB2CCBF82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{52AC3B38-E3FD-44E8-974D-300D6821E957}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{52AC3B38-E3FD-44E8-974D-300D6821E957}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Identity" sheetId="1" r:id="rId1"/>
+    <sheet name="Application" sheetId="2" r:id="rId2"/>
+    <sheet name="Link" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="85">
   <si>
     <t>Return Type</t>
   </si>
@@ -201,6 +203,96 @@
   </si>
   <si>
     <t>getAttribute("attributeName")</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>getApplication()</t>
+  </si>
+  <si>
+    <t>Application where the account resides.</t>
+  </si>
+  <si>
+    <t>getApplicationId()</t>
+  </si>
+  <si>
+    <t>Gets the id of the application referenced by this link.</t>
+  </si>
+  <si>
+    <t>getApplicationName()</t>
+  </si>
+  <si>
+    <t>Gets the name of the application referenced by this link.</t>
+  </si>
+  <si>
+    <t>getAttribute(attributeName)</t>
+  </si>
+  <si>
+    <t>Gets a specific attribute value from the Link</t>
+  </si>
+  <si>
+    <t>Gets all the attributes associated with the Link</t>
+  </si>
+  <si>
+    <t>getIdentity()</t>
+  </si>
+  <si>
+    <t>Gets owning Identity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getIiqDisabled() </t>
+  </si>
+  <si>
+    <t xml:space="preserve">getIiqLocked() </t>
+  </si>
+  <si>
+    <t>True if link is disabled</t>
+  </si>
+  <si>
+    <t>true if link is locked</t>
+  </si>
+  <si>
+    <t>The "raw" account identity.</t>
+  </si>
+  <si>
+    <t>getNativeIdentity()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isDisabled() </t>
+  </si>
+  <si>
+    <t xml:space="preserve">isLocked() </t>
+  </si>
+  <si>
+    <t>isManuallyCorrelated()</t>
+  </si>
+  <si>
+    <t>setAttribute(name, value)</t>
+  </si>
+  <si>
+    <t>Sets an attribute to the link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">setIiqDisabled() </t>
+  </si>
+  <si>
+    <t xml:space="preserve">setIiqLocked() </t>
+  </si>
+  <si>
+    <t>Sets link as disabled status</t>
+  </si>
+  <si>
+    <t>sets link as locked status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">setManuallyCorrelated(boolean manual) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">setNativeIdentity(String id) </t>
+  </si>
+  <si>
+    <t>Flag to indicate account was manually correlated in the UI and the identity association should be left as is.</t>
   </si>
 </sst>
 </file>
@@ -269,11 +361,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,18 +685,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542FAFEE-048F-4B99-88D3-83834E0D810F}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,7 +707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -623,7 +718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -634,7 +729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -645,7 +740,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -656,7 +751,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -667,7 +762,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -678,7 +773,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -689,7 +784,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -700,7 +795,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -711,7 +806,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -722,7 +817,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -733,7 +828,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -744,7 +839,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -755,7 +850,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
@@ -766,7 +861,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
@@ -777,7 +872,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -788,7 +883,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>39</v>
       </c>
@@ -799,7 +894,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>39</v>
       </c>
@@ -810,7 +905,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>39</v>
       </c>
@@ -821,7 +916,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>39</v>
       </c>
@@ -832,7 +927,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>39</v>
       </c>
@@ -843,7 +938,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>39</v>
       </c>
@@ -863,4 +958,229 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB718F01-6F54-4230-A2A7-5B1CE68E5247}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70300212-E139-4815-8F88-3FAE633B1ADE}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>